<commit_message>
updates to creating figures
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_ACTIVE_P2.xlsx
+++ b/rmonize/data_proc_elem/DPE_ACTIVE_P2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\rmonize\data_proc_elem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{227E31C3-C779-4E6E-8B11-0E7E931415C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FADCA61C-1225-4534-AF08-75A2A880A75B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="22290" windowHeight="12000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="305">
   <si>
     <t>index</t>
   </si>
@@ -1070,7 +1070,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1086,9 +1086,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1126,9 +1126,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1161,9 +1161,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1196,9 +1213,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1374,13 +1408,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="E97" workbookViewId="0">
+      <selection activeCell="J94" sqref="J94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="6" width="27.90625" customWidth="1"/>
+    <col min="7" max="7" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.1796875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1415,7 +1454,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1447,7 +1486,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1479,7 +1518,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1511,7 +1550,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1543,7 +1582,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1575,7 +1614,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1610,7 +1649,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1642,7 +1681,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1674,7 +1713,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1706,7 +1745,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1741,7 +1780,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1773,7 +1812,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1805,7 +1844,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1834,7 +1873,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1866,7 +1905,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1898,7 +1937,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1927,7 +1966,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1956,7 +1995,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1985,7 +2024,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2007,8 +2046,11 @@
       <c r="I20" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2040,7 +2082,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2072,7 +2114,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2104,7 +2146,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2136,7 +2178,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2165,7 +2207,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2197,7 +2239,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2229,7 +2271,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2258,7 +2300,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2287,7 +2329,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2316,7 +2358,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2345,7 +2387,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2374,7 +2416,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2403,7 +2445,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2432,7 +2474,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2461,7 +2503,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2490,7 +2532,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2519,7 +2561,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2551,7 +2593,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2580,7 +2622,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2609,7 +2651,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2638,7 +2680,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2667,7 +2709,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2696,7 +2738,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2725,7 +2767,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2754,7 +2796,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2783,7 +2825,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2812,7 +2854,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2841,7 +2883,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2870,7 +2912,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2899,7 +2941,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2928,7 +2970,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2957,7 +2999,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2986,7 +3028,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3015,7 +3057,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3044,7 +3086,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>55</v>
       </c>
@@ -3073,7 +3115,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>56</v>
       </c>
@@ -3102,7 +3144,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3131,7 +3173,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3160,7 +3202,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3189,7 +3231,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3218,7 +3260,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3247,7 +3289,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>62</v>
       </c>
@@ -3276,7 +3318,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>63</v>
       </c>
@@ -3305,7 +3347,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>64</v>
       </c>
@@ -3334,7 +3376,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>65</v>
       </c>
@@ -3366,7 +3408,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>66</v>
       </c>
@@ -3395,7 +3437,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>67</v>
       </c>
@@ -3424,7 +3466,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>68</v>
       </c>
@@ -3453,7 +3495,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>69</v>
       </c>
@@ -3482,7 +3524,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>70</v>
       </c>
@@ -3514,7 +3556,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>71</v>
       </c>
@@ -3546,7 +3588,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>72</v>
       </c>
@@ -3575,7 +3617,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>73</v>
       </c>
@@ -3604,7 +3646,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>74</v>
       </c>
@@ -3636,7 +3678,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>75</v>
       </c>
@@ -3665,7 +3707,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>76</v>
       </c>
@@ -3697,7 +3739,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>77</v>
       </c>
@@ -3726,7 +3768,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>78</v>
       </c>
@@ -3758,7 +3800,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>79</v>
       </c>
@@ -3790,7 +3832,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>80</v>
       </c>
@@ -3822,7 +3864,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>81</v>
       </c>
@@ -3854,7 +3896,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>82</v>
       </c>
@@ -3886,7 +3928,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>83</v>
       </c>
@@ -3918,7 +3960,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>84</v>
       </c>
@@ -3950,7 +3992,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>85</v>
       </c>
@@ -3979,7 +4021,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>86</v>
       </c>
@@ -4011,7 +4053,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>87</v>
       </c>
@@ -4043,7 +4085,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>88</v>
       </c>
@@ -4065,8 +4107,11 @@
       <c r="I89" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J89" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>89</v>
       </c>
@@ -4088,8 +4133,11 @@
       <c r="I90" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J90" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>90</v>
       </c>
@@ -4111,8 +4159,11 @@
       <c r="I91" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J91" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>91</v>
       </c>
@@ -4134,8 +4185,11 @@
       <c r="I92" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J92" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>92</v>
       </c>
@@ -4157,8 +4211,11 @@
       <c r="I93" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J93" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>93</v>
       </c>
@@ -4180,8 +4237,11 @@
       <c r="I94" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J94" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>94</v>
       </c>
@@ -4213,7 +4273,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>95</v>
       </c>
@@ -4245,7 +4305,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>96</v>
       </c>
@@ -4277,7 +4337,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>97</v>
       </c>
@@ -4309,7 +4369,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>98</v>
       </c>
@@ -4341,7 +4401,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>99</v>
       </c>
@@ -4373,7 +4433,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>100</v>
       </c>
@@ -4405,7 +4465,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>101</v>
       </c>
@@ -4437,7 +4497,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>102</v>
       </c>
@@ -4469,7 +4529,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>103</v>
       </c>
@@ -4501,7 +4561,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>104</v>
       </c>
@@ -4533,7 +4593,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>105</v>
       </c>
@@ -4565,7 +4625,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>106</v>
       </c>
@@ -4597,7 +4657,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>107</v>
       </c>
@@ -4629,7 +4689,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>108</v>
       </c>

</xml_diff>